<commit_message>
Commiting day3 Final Assignment,consisting of api automation scripts via pytest and passed run reports
</commit_message>
<xml_diff>
--- a/API_Data.xlsx
+++ b/API_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amedeloitte-my.sharepoint.com/personal/firdi_deloitte_com/Documents/Training/Api_final_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{82CEB8ED-EE7E-C24E-BC24-5B6BEE641386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68F5B5E4-8164-DF44-9F73-73A03DC46A39}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{82CEB8ED-EE7E-C24E-BC24-5B6BEE641386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D05C9AD-AF52-2142-A218-6E0B5C4092CE}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>password</t>
   </si>
@@ -93,9 +93,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Shaikhh Test</t>
-  </si>
-  <si>
     <t>Add20Tasks</t>
   </si>
   <si>
@@ -213,7 +210,46 @@
     <t>200000</t>
   </si>
   <si>
-    <t>shaik59@test.com</t>
+    <t>Adding_20_tasks</t>
+  </si>
+  <si>
+    <t>Shaikh Test</t>
+  </si>
+  <si>
+    <t>Shaikhh</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>task17</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Register_f</t>
+  </si>
+  <si>
+    <t>Login_f</t>
+  </si>
+  <si>
+    <t>Test_Func</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>register@test.com</t>
+  </si>
+  <si>
+    <t>testhash39@test.com</t>
+  </si>
+  <si>
+    <t>taprt29816@test.com</t>
   </si>
 </sst>
 </file>
@@ -586,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5752FA-5421-0E44-B733-D04398AC9CA1}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +642,7 @@
     <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -632,15 +668,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -650,13 +686,15 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -666,7 +704,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -682,7 +720,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -701,7 +739,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -712,134 +750,191 @@
         <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="I6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="U12" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>58</v>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -847,6 +942,9 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{AEADA043-665E-AB41-A68C-4813DF4B4CD0}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{808D7ED5-34AB-D742-AB05-83C9FCEECE21}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{57F1C537-FEBB-D042-8B39-5AADC27CA033}"/>
+    <hyperlink ref="C14" r:id="rId4" xr:uid="{3769E624-D49A-7B48-9066-C849D4C63C85}"/>
+    <hyperlink ref="C15" r:id="rId5" xr:uid="{F5823DA7-4748-0049-9182-2EA2F1D6E03E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>